<commit_message>
added the buffer layer to the TAPD model
</commit_message>
<xml_diff>
--- a/doc/AtomicRadii.xlsx
+++ b/doc/AtomicRadii.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yux20\Documents\PyRHEED\Source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yux20\Documents\PyRHEED\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBBA01B-4E44-46D4-B6B1-B911419E162F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA7C6CB-D5E5-4C60-B5D7-97E3B9DADC2A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="1" xr2:uid="{48EF06C2-012D-4792-9077-5E72BCB4E015}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="1" xr2:uid="{48EF06C2-012D-4792-9077-5E72BCB4E015}"/>
   </bookViews>
   <sheets>
     <sheet name="Crystal Radius" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="116">
   <si>
     <t>H</t>
   </si>
@@ -344,6 +344,57 @@
   </si>
   <si>
     <t>Np</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>FFFFFF</t>
+  </si>
+  <si>
+    <t>00FF00</t>
+  </si>
+  <si>
+    <t>FFC0CB</t>
+  </si>
+  <si>
+    <t>B22222</t>
+  </si>
+  <si>
+    <t>FF1493</t>
+  </si>
+  <si>
+    <t>C8C8C8</t>
+  </si>
+  <si>
+    <t>8F8FFF</t>
+  </si>
+  <si>
+    <t>F00000</t>
+  </si>
+  <si>
+    <t>DAA520</t>
+  </si>
+  <si>
+    <t>0000FF</t>
+  </si>
+  <si>
+    <t>228B22</t>
+  </si>
+  <si>
+    <t>808090</t>
+  </si>
+  <si>
+    <t>FFA500</t>
+  </si>
+  <si>
+    <t>FFC832</t>
+  </si>
+  <si>
+    <t>A52A2A</t>
+  </si>
+  <si>
+    <t>A020F0</t>
   </si>
 </sst>
 </file>
@@ -379,12 +430,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1858,1144 +1915,1427 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5B26D2-EDF5-4C61-AC42-6AF69AC00B59}">
-  <dimension ref="A1:C94"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>0.53</v>
       </c>
-      <c r="C2" s="2">
-        <f>B2/MAX(B2:B94)*60</f>
+      <c r="C2" s="4">
+        <f t="shared" ref="C2:C33" si="0">B2/MAX(B2:B94)*60</f>
         <v>10.671140939597317</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>93</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>0.31</v>
       </c>
-      <c r="C3" s="2">
-        <f>B3/MAX(B3:B95)*60</f>
+      <c r="C3" s="4">
+        <f t="shared" si="0"/>
         <v>6.2416107382550337</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>1.67</v>
       </c>
-      <c r="C4" s="2">
-        <f>B4/MAX(B4:B96)*60</f>
+      <c r="C4" s="4">
+        <f t="shared" si="0"/>
         <v>33.624161073825505</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C5" s="2">
-        <f>B5/MAX(B5:B97)*60</f>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
         <v>22.550335570469798</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>0.87</v>
       </c>
-      <c r="C6" s="2">
-        <f>B6/MAX(B6:B98)*60</f>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
         <v>17.516778523489933</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>0.67</v>
       </c>
-      <c r="C7" s="2">
-        <f>B7/MAX(B7:B99)*60</f>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
         <v>13.489932885906041</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>0.56000000000000005</v>
       </c>
-      <c r="C8" s="2">
-        <f>B8/MAX(B8:B100)*60</f>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
         <v>11.275167785234899</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>0.48</v>
       </c>
-      <c r="C9" s="2">
-        <f>B9/MAX(B9:B101)*60</f>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
         <v>9.6644295302013425</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>0.42</v>
       </c>
-      <c r="C10" s="2">
-        <f>B10/MAX(B10:B102)*60</f>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
         <v>8.4563758389261743</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>94</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>0.38</v>
       </c>
-      <c r="C11" s="2">
-        <f>B11/MAX(B11:B103)*60</f>
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
         <v>7.6510067114093969</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>1.9</v>
       </c>
-      <c r="C12" s="2">
-        <f>B12/MAX(B12:B104)*60</f>
+      <c r="C12" s="4">
+        <f t="shared" si="0"/>
         <v>38.255033557046978</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>1.45</v>
       </c>
-      <c r="C13" s="2">
-        <f>B13/MAX(B13:B105)*60</f>
+      <c r="C13" s="4">
+        <f t="shared" si="0"/>
         <v>29.19463087248322</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>1.18</v>
       </c>
-      <c r="C14" s="2">
-        <f>B14/MAX(B14:B106)*60</f>
+      <c r="C14" s="4">
+        <f t="shared" si="0"/>
         <v>23.758389261744966</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>1.1100000000000001</v>
       </c>
-      <c r="C15" s="2">
-        <f>B15/MAX(B15:B107)*60</f>
+      <c r="C15" s="4">
+        <f t="shared" si="0"/>
         <v>22.348993288590606</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>0.98</v>
       </c>
-      <c r="C16" s="2">
-        <f>B16/MAX(B16:B108)*60</f>
+      <c r="C16" s="4">
+        <f t="shared" si="0"/>
         <v>19.731543624161073</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>0.88</v>
       </c>
-      <c r="C17" s="2">
-        <f>B17/MAX(B17:B109)*60</f>
+      <c r="C17" s="4">
+        <f t="shared" si="0"/>
         <v>17.718120805369129</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="3">
         <v>0.79</v>
       </c>
-      <c r="C18" s="2">
-        <f>B18/MAX(B18:B110)*60</f>
+      <c r="C18" s="4">
+        <f t="shared" si="0"/>
         <v>15.906040268456376</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>95</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="3">
         <v>0.71</v>
       </c>
-      <c r="C19" s="2">
-        <f>B19/MAX(B19:B111)*60</f>
+      <c r="C19" s="4">
+        <f t="shared" si="0"/>
         <v>14.295302013422818</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="3">
         <v>2.4300000000000002</v>
       </c>
-      <c r="C20" s="2">
-        <f>B20/MAX(B20:B112)*60</f>
+      <c r="C20" s="4">
+        <f t="shared" si="0"/>
         <v>48.9261744966443</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="3">
         <v>1.94</v>
       </c>
-      <c r="C21" s="2">
-        <f>B21/MAX(B21:B113)*60</f>
+      <c r="C21" s="4">
+        <f t="shared" si="0"/>
         <v>39.060402684563755</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="3">
         <v>1.84</v>
       </c>
-      <c r="C22" s="2">
-        <f>B22/MAX(B22:B114)*60</f>
+      <c r="C22" s="4">
+        <f t="shared" si="0"/>
         <v>37.04697986577181</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="3">
         <v>1.76</v>
       </c>
-      <c r="C23" s="2">
-        <f>B23/MAX(B23:B115)*60</f>
+      <c r="C23" s="4">
+        <f t="shared" si="0"/>
         <v>35.436241610738257</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="3">
         <v>1.71</v>
       </c>
-      <c r="C24" s="2">
-        <f>B24/MAX(B24:B116)*60</f>
+      <c r="C24" s="4">
+        <f t="shared" si="0"/>
         <v>34.429530201342281</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="3">
         <v>1.66</v>
       </c>
-      <c r="C25" s="2">
-        <f>B25/MAX(B25:B117)*60</f>
+      <c r="C25" s="4">
+        <f t="shared" si="0"/>
         <v>33.422818791946305</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="3">
         <v>1.61</v>
       </c>
-      <c r="C26" s="2">
-        <f>B26/MAX(B26:B118)*60</f>
+      <c r="C26" s="4">
+        <f t="shared" si="0"/>
         <v>32.416107382550337</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>22</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="3">
         <v>1.56</v>
       </c>
-      <c r="C27" s="2">
-        <f>B27/MAX(B27:B119)*60</f>
+      <c r="C27" s="4">
+        <f t="shared" si="0"/>
         <v>31.409395973154364</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>23</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="3">
         <v>1.52</v>
       </c>
-      <c r="C28" s="2">
-        <f>B28/MAX(B28:B120)*60</f>
+      <c r="C28" s="4">
+        <f t="shared" si="0"/>
         <v>30.604026845637588</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>24</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="3">
         <v>1.49</v>
       </c>
-      <c r="C29" s="2">
-        <f>B29/MAX(B29:B121)*60</f>
+      <c r="C29" s="4">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>25</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="3">
         <v>1.45</v>
       </c>
-      <c r="C30" s="2">
-        <f>B30/MAX(B30:B122)*60</f>
+      <c r="C30" s="4">
+        <f t="shared" si="0"/>
         <v>29.19463087248322</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>26</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="3">
         <v>1.42</v>
       </c>
-      <c r="C31" s="2">
-        <f>B31/MAX(B31:B123)*60</f>
+      <c r="C31" s="4">
+        <f t="shared" si="0"/>
         <v>28.590604026845636</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>27</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="3">
         <v>1.36</v>
       </c>
-      <c r="C32" s="2">
-        <f>B32/MAX(B32:B124)*60</f>
+      <c r="C32" s="4">
+        <f t="shared" si="0"/>
         <v>27.382550335570475</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>28</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="3">
         <v>1.25</v>
       </c>
-      <c r="C33" s="2">
-        <f>B33/MAX(B33:B125)*60</f>
+      <c r="C33" s="4">
+        <f t="shared" si="0"/>
         <v>25.167785234899331</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>29</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="3">
         <v>1.1399999999999999</v>
       </c>
-      <c r="C34" s="2">
-        <f>B34/MAX(B34:B126)*60</f>
+      <c r="C34" s="4">
+        <f t="shared" ref="C34:C65" si="1">B34/MAX(B34:B126)*60</f>
         <v>22.953020134228186</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>30</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="3">
         <v>1.03</v>
       </c>
-      <c r="C35" s="2">
-        <f>B35/MAX(B35:B127)*60</f>
+      <c r="C35" s="4">
+        <f t="shared" si="1"/>
         <v>20.738255033557046</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>31</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="3">
         <v>0.94</v>
       </c>
-      <c r="C36" s="2">
-        <f>B36/MAX(B36:B128)*60</f>
+      <c r="C36" s="4">
+        <f t="shared" si="1"/>
         <v>18.926174496644293</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>96</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="3">
         <v>0.88</v>
       </c>
-      <c r="C37" s="2">
-        <f>B37/MAX(B37:B129)*60</f>
+      <c r="C37" s="4">
+        <f t="shared" si="1"/>
         <v>17.718120805369129</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="3">
         <v>2.65</v>
       </c>
-      <c r="C38" s="2">
-        <f>B38/MAX(B38:B130)*60</f>
+      <c r="C38" s="4">
+        <f t="shared" si="1"/>
         <v>53.355704697986575</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="3">
         <v>2.19</v>
       </c>
-      <c r="C39" s="2">
-        <f>B39/MAX(B39:B131)*60</f>
+      <c r="C39" s="4">
+        <f t="shared" si="1"/>
         <v>44.09395973154362</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>34</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="3">
         <v>2.12</v>
       </c>
-      <c r="C40" s="2">
-        <f>B40/MAX(B40:B132)*60</f>
+      <c r="C40" s="4">
+        <f t="shared" si="1"/>
         <v>42.684563758389267</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="3">
         <v>2.06</v>
       </c>
-      <c r="C41" s="2">
-        <f>B41/MAX(B41:B133)*60</f>
+      <c r="C41" s="4">
+        <f t="shared" si="1"/>
         <v>41.476510067114091</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>36</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="3">
         <v>1.98</v>
       </c>
-      <c r="C42" s="2">
-        <f>B42/MAX(B42:B134)*60</f>
+      <c r="C42" s="4">
+        <f t="shared" si="1"/>
         <v>39.865771812080538</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>37</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="3">
         <v>1.9</v>
       </c>
-      <c r="C43" s="2">
-        <f>B43/MAX(B43:B135)*60</f>
+      <c r="C43" s="4">
+        <f t="shared" si="1"/>
         <v>38.255033557046978</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>38</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="3">
         <v>1.83</v>
       </c>
-      <c r="C44" s="2">
-        <f>B44/MAX(B44:B136)*60</f>
+      <c r="C44" s="4">
+        <f t="shared" si="1"/>
         <v>36.845637583892618</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>39</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="3">
         <v>1.78</v>
       </c>
-      <c r="C45" s="2">
-        <f>B45/MAX(B45:B137)*60</f>
+      <c r="C45" s="4">
+        <f t="shared" si="1"/>
         <v>35.838926174496649</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>40</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="3">
         <v>1.73</v>
       </c>
-      <c r="C46" s="2">
-        <f>B46/MAX(B46:B138)*60</f>
+      <c r="C46" s="4">
+        <f t="shared" si="1"/>
         <v>34.832214765100673</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>41</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="3">
         <v>1.69</v>
       </c>
-      <c r="C47" s="2">
-        <f>B47/MAX(B47:B139)*60</f>
+      <c r="C47" s="4">
+        <f t="shared" si="1"/>
         <v>34.026845637583897</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>42</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="3">
         <v>1.65</v>
       </c>
-      <c r="C48" s="2">
-        <f>B48/MAX(B48:B140)*60</f>
+      <c r="C48" s="4">
+        <f t="shared" si="1"/>
         <v>33.221476510067106</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>43</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="3">
         <v>1.61</v>
       </c>
-      <c r="C49" s="2">
-        <f>B49/MAX(B49:B141)*60</f>
+      <c r="C49" s="4">
+        <f t="shared" si="1"/>
         <v>32.416107382550337</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>44</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="3">
         <v>1.56</v>
       </c>
-      <c r="C50" s="2">
-        <f>B50/MAX(B50:B142)*60</f>
+      <c r="C50" s="4">
+        <f t="shared" si="1"/>
         <v>31.409395973154364</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>45</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="3">
         <v>1.45</v>
       </c>
-      <c r="C51" s="2">
-        <f>B51/MAX(B51:B143)*60</f>
+      <c r="C51" s="4">
+        <f t="shared" si="1"/>
         <v>29.19463087248322</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>46</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="3">
         <v>1.33</v>
       </c>
-      <c r="C52" s="2">
-        <f>B52/MAX(B52:B144)*60</f>
+      <c r="C52" s="4">
+        <f t="shared" si="1"/>
         <v>26.778523489932887</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>47</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="3">
         <v>1.23</v>
       </c>
-      <c r="C53" s="2">
-        <f>B53/MAX(B53:B145)*60</f>
+      <c r="C53" s="4">
+        <f t="shared" si="1"/>
         <v>24.765100671140942</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>48</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="3">
         <v>1.1499999999999999</v>
       </c>
-      <c r="C54" s="2">
-        <f>B54/MAX(B54:B146)*60</f>
+      <c r="C54" s="4">
+        <f t="shared" si="1"/>
         <v>23.154362416107382</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>49</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="3">
         <v>1.08</v>
       </c>
-      <c r="C55" s="2">
-        <f>B55/MAX(B55:B147)*60</f>
+      <c r="C55" s="4">
+        <f t="shared" si="1"/>
         <v>21.744966442953022</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>50</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="3">
         <v>2.98</v>
       </c>
-      <c r="C56" s="2">
-        <f>B56/MAX(B56:B148)*60</f>
+      <c r="C56" s="4">
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>51</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="3">
         <v>2.5299999999999998</v>
       </c>
-      <c r="C57" s="2">
-        <f>B57/MAX(B57:B149)*60</f>
+      <c r="C57" s="4">
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>52</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="3">
         <v>1.95</v>
       </c>
-      <c r="C58" s="2">
-        <f>B58/MAX(B58:B150)*60</f>
+      <c r="C58" s="4">
+        <f t="shared" si="1"/>
         <v>47.368421052631575</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>53</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="3">
         <v>1.85</v>
       </c>
-      <c r="C59" s="2">
-        <f>B59/MAX(B59:B151)*60</f>
+      <c r="C59" s="4">
+        <f t="shared" si="1"/>
         <v>44.939271255060724</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>54</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="3">
         <v>2.4700000000000002</v>
       </c>
-      <c r="C60" s="2">
-        <f>B60/MAX(B60:B152)*60</f>
+      <c r="C60" s="4">
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>55</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="3">
         <v>2.06</v>
       </c>
-      <c r="C61" s="2">
-        <f>B61/MAX(B61:B153)*60</f>
+      <c r="C61" s="4">
+        <f t="shared" si="1"/>
         <v>51.932773109243698</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>56</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="3">
         <v>2.0499999999999998</v>
       </c>
-      <c r="C62" s="2">
-        <f>B62/MAX(B62:B154)*60</f>
+      <c r="C62" s="4">
+        <f t="shared" si="1"/>
         <v>51.680672268907557</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>57</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="3">
         <v>2.38</v>
       </c>
-      <c r="C63" s="2">
-        <f>B63/MAX(B63:B155)*60</f>
+      <c r="C63" s="4">
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>58</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="3">
         <v>2.31</v>
       </c>
-      <c r="C64" s="2">
-        <f>B64/MAX(B64:B156)*60</f>
+      <c r="C64" s="4">
+        <f t="shared" si="1"/>
         <v>59.484978540772531</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>59</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="3">
         <v>2.33</v>
       </c>
-      <c r="C65" s="2">
-        <f>B65/MAX(B65:B157)*60</f>
+      <c r="C65" s="4">
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>60</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="3">
         <v>2.25</v>
       </c>
-      <c r="C66" s="2">
-        <f>B66/MAX(B66:B158)*60</f>
+      <c r="C66" s="4">
+        <f t="shared" ref="C66:C97" si="2">B66/MAX(B66:B158)*60</f>
         <v>59.21052631578948</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>61</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="3">
         <v>2.2799999999999998</v>
       </c>
-      <c r="C67" s="2">
-        <f>B67/MAX(B67:B159)*60</f>
+      <c r="C67" s="4">
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>62</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="3">
         <v>2.2599999999999998</v>
       </c>
-      <c r="C68" s="2">
-        <f>B68/MAX(B68:B160)*60</f>
+      <c r="C68" s="4">
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>63</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="3">
         <v>2.2599999999999998</v>
       </c>
-      <c r="C69" s="2">
-        <f>B69/MAX(B69:B161)*60</f>
+      <c r="C69" s="4">
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>64</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="3">
         <v>2.2200000000000002</v>
       </c>
-      <c r="C70" s="2">
-        <f>B70/MAX(B70:B162)*60</f>
+      <c r="C70" s="4">
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>65</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="3">
         <v>2.2200000000000002</v>
       </c>
-      <c r="C71" s="2">
-        <f>B71/MAX(B71:B163)*60</f>
+      <c r="C71" s="4">
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>66</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="3">
         <v>2.17</v>
       </c>
-      <c r="C72" s="2">
-        <f>B72/MAX(B72:B164)*60</f>
+      <c r="C72" s="4">
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>67</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="3">
         <v>2.08</v>
       </c>
-      <c r="C73" s="2">
-        <f>B73/MAX(B73:B165)*60</f>
+      <c r="C73" s="4">
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>68</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="3">
         <v>2</v>
       </c>
-      <c r="C74" s="2">
-        <f>B74/MAX(B74:B166)*60</f>
+      <c r="C74" s="4">
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>69</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="3">
         <v>1.93</v>
       </c>
-      <c r="C75" s="2">
-        <f>B75/MAX(B75:B167)*60</f>
+      <c r="C75" s="4">
+        <f t="shared" si="2"/>
         <v>59.384615384615387</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>70</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="3">
         <v>1.88</v>
       </c>
-      <c r="C76" s="2">
-        <f>B76/MAX(B76:B168)*60</f>
+      <c r="C76" s="4">
+        <f t="shared" si="2"/>
         <v>57.846153846153847</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>71</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="3">
         <v>1.85</v>
       </c>
-      <c r="C77" s="2">
-        <f>B77/MAX(B77:B169)*60</f>
+      <c r="C77" s="4">
+        <f t="shared" si="2"/>
         <v>56.923076923076927</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>72</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="3">
         <v>1.8</v>
       </c>
-      <c r="C78" s="2">
-        <f>B78/MAX(B78:B170)*60</f>
+      <c r="C78" s="4">
+        <f t="shared" si="2"/>
         <v>55.384615384615387</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>73</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="3">
         <v>1.77</v>
       </c>
-      <c r="C79" s="2">
-        <f>B79/MAX(B79:B171)*60</f>
+      <c r="C79" s="4">
+        <f t="shared" si="2"/>
         <v>54.46153846153846</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>74</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="3">
         <v>1.74</v>
       </c>
-      <c r="C80" s="2">
-        <f>B80/MAX(B80:B172)*60</f>
+      <c r="C80" s="4">
+        <f t="shared" si="2"/>
         <v>53.53846153846154</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>75</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="3">
         <v>1.71</v>
       </c>
-      <c r="C81" s="2">
-        <f>B81/MAX(B81:B173)*60</f>
+      <c r="C81" s="4">
+        <f t="shared" si="2"/>
         <v>52.615384615384613</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>76</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="3">
         <v>1.56</v>
       </c>
-      <c r="C82" s="2">
-        <f>B82/MAX(B82:B174)*60</f>
+      <c r="C82" s="4">
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>77</v>
       </c>
-      <c r="B83">
+      <c r="B83" s="3">
         <v>1.54</v>
       </c>
-      <c r="C83" s="2">
-        <f>B83/MAX(B83:B175)*60</f>
+      <c r="C83" s="4">
+        <f t="shared" si="2"/>
         <v>47.384615384615387</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>78</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="3">
         <v>1.43</v>
       </c>
-      <c r="C84" s="2">
-        <f>B84/MAX(B84:B176)*60</f>
+      <c r="C84" s="4">
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>79</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="3">
         <v>1.35</v>
       </c>
-      <c r="C85" s="2">
-        <f>B85/MAX(B85:B177)*60</f>
+      <c r="C85" s="4">
+        <f t="shared" si="2"/>
         <v>41.538461538461547</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>80</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="3">
         <v>1.27</v>
       </c>
-      <c r="C86" s="2">
-        <f>B86/MAX(B86:B178)*60</f>
+      <c r="C86" s="4">
+        <f t="shared" si="2"/>
         <v>39.07692307692308</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>97</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="3">
         <v>1.2</v>
       </c>
-      <c r="C87" s="2">
-        <f>B87/MAX(B87:B179)*60</f>
+      <c r="C87" s="4">
+        <f t="shared" si="2"/>
         <v>36.923076923076927</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>83</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="3">
         <v>1.95</v>
       </c>
-      <c r="C88" s="2">
-        <f>B88/MAX(B88:B182)*60</f>
+      <c r="C88" s="4">
+        <f t="shared" ref="C88:C94" si="3">B88/MAX(B88:B182)*60</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>84</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="3">
         <v>1.8</v>
       </c>
-      <c r="C89" s="2">
-        <f>B89/MAX(B89:B183)*60</f>
+      <c r="C89" s="4">
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>85</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="3">
         <v>1.8</v>
       </c>
-      <c r="C90" s="2">
-        <f>B90/MAX(B90:B184)*60</f>
+      <c r="C90" s="4">
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>86</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="3">
         <v>1.75</v>
       </c>
-      <c r="C91" s="2">
-        <f>B91/MAX(B91:B185)*60</f>
+      <c r="C91" s="4">
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>98</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="3">
         <v>1.75</v>
       </c>
-      <c r="C92" s="2">
-        <f>B92/MAX(B92:B186)*60</f>
+      <c r="C92" s="4">
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>87</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="3">
         <v>1.75</v>
       </c>
-      <c r="C93" s="2">
-        <f>B93/MAX(B93:B187)*60</f>
+      <c r="C93" s="4">
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>88</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="3">
         <v>1.75</v>
       </c>
-      <c r="C94" s="2">
-        <f>B94/MAX(B94:B188)*60</f>
+      <c r="C94" s="4">
+        <f t="shared" si="3"/>
         <v>60</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>